<commit_message>
added dependency, added test, removed junk from input file, incremented patch version
</commit_message>
<xml_diff>
--- a/adapter/tests/test_w_inputs_from_files_table_sqlalchemy.xlsx
+++ b/adapter/tests/test_w_inputs_from_files_table_sqlalchemy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\tburke\documents\aptana studio 3 workspace\adapter\adapter\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrahovac/repos/adapter/adapter/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF29404-A3D0-4E4A-A641-3771A834D244}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10110" windowHeight="10490"/>
+    <workbookView xWindow="51960" yWindow="1360" windowWidth="27720" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test - Copy" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Output Path</t>
   </si>
@@ -94,9 +95,6 @@
   </si>
   <si>
     <t>Y, Y, Y</t>
-  </si>
-  <si>
-    <t>{table1:db_con, table2:db_con, table3:db_con}</t>
   </si>
   <si>
     <t>adapter_example_table1, adapter_example_table2, adapter_example_table3</t>
@@ -108,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,47 +646,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="xlsx_table15" displayName="xlsx_table15" ref="J2:L5" totalsRowShown="0">
-  <autoFilter ref="J2:L5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="xlsx_table15" displayName="xlsx_table15" ref="J2:L5" totalsRowShown="0">
+  <autoFilter ref="J2:L5" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col_1"/>
-    <tableColumn id="2" name="col_2"/>
-    <tableColumn id="3" name="col_3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="col_1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="col_2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="col_3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="xlsx_table26" displayName="xlsx_table26" ref="J9:L12" totalsRowShown="0">
-  <autoFilter ref="J9:L12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="xlsx_table26" displayName="xlsx_table26" ref="J9:L12" totalsRowShown="0">
+  <autoFilter ref="J9:L12" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col_11"/>
-    <tableColumn id="2" name="col_22"/>
-    <tableColumn id="3" name="col_33"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="col_11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="col_22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="col_33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
-  <autoFilter ref="B2:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Output Path"/>
-    <tableColumn id="2" name="Version"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Output Path"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="inputs_from_files" displayName="inputs_from_files" ref="B7:D11" totalsRowShown="0">
-  <autoFilter ref="B7:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="inputs_from_files" displayName="inputs_from_files" ref="B7:D11" totalsRowShown="0">
+  <autoFilter ref="B7:D11" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="File Path"/>
-    <tableColumn id="2" name="Table Name"/>
-    <tableColumn id="3" name="Query Only"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="File Path"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Table Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Query Only"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -956,21 +954,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="55.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -987,7 +985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J4">
         <v>1</v>
       </c>
@@ -1015,7 +1013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J5">
         <v>1</v>
       </c>
@@ -1026,7 +1024,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -1048,7 +1046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1062,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -1076,12 +1074,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -1096,7 +1094,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J12">
         <v>11</v>
       </c>
@@ -1105,11 +1103,6 @@
       </c>
       <c r="L12">
         <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tested haggis connection and added comment to its test input
</commit_message>
<xml_diff>
--- a/adapter/tests/test_w_inputs_from_files_table_sqlalchemy.xlsx
+++ b/adapter/tests/test_w_inputs_from_files_table_sqlalchemy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrahovac/repos/adapter/adapter/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/mgrahovac/repos/adapter/adapter/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF29404-A3D0-4E4A-A641-3771A834D244}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5439BE3-29AE-6042-8B1A-67C5B04805C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51960" yWindow="1360" windowWidth="27720" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Output Path</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>haggis.lbl.gov/lcc_adapter</t>
+  </si>
+  <si>
+    <t>*Table Name must be provided for server readin</t>
   </si>
 </sst>
 </file>
@@ -958,7 +961,7 @@
   <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1084,6 +1087,9 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
       <c r="J11">
         <v>11</v>
       </c>

</xml_diff>